<commit_message>
[#2] update ignore and work hours
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,19 +371,41 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <f aca="false">(C5&lt;B5)+C5-B5</f>
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <f aca="false">(D5*24)*E5</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="n">
-        <f aca="false">SUM(D2:D4)</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="n">
-        <f aca="false">SUM(F2:F4)</f>
-        <v>80</v>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="n">
+        <f aca="false">SUM(D2:D5)</f>
+        <v>0.583333333333333</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="n">
+        <f aca="false">SUM(F2:F5)</f>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#2] Update work hours
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -275,10 +275,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -378,18 +378,18 @@
         <v>0.625</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>0.875</v>
+        <v>0.958333333333333</v>
       </c>
       <c r="D5" s="8" t="n">
         <f aca="false">(C5&lt;B5)+C5-B5</f>
-        <v>0.25</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>10</v>
       </c>
       <c r="F5" s="9" t="n">
         <f aca="false">(D5*24)*E5</f>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,12 +400,12 @@
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="n">
         <f aca="false">SUM(D2:D5)</f>
-        <v>0.583333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="n">
         <f aca="false">SUM(F2:F5)</f>
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#2][#7][#8] Store and render images and reviews from database
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -393,19 +393,41 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <f aca="false">(C6&lt;B6)+C6-B6</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <f aca="false">(D6*24)*E6</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12" t="n">
-        <f aca="false">SUM(D2:D5)</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="n">
-        <f aca="false">SUM(F2:F5)</f>
-        <v>160</v>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12" t="n">
+        <f aca="false">SUM(D2:D6)</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="n">
+        <f aca="false">SUM(F2:F6)</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#9] Added button to '/reviews' on home page
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -415,19 +415,41 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="n">
+        <v>45269</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <f aca="false">(C7&lt;B7)+C7-B7</f>
+        <v>0.375</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="n">
+        <f aca="false">(D7*24)*E7</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12" t="n">
-        <f aca="false">SUM(D2:D6)</f>
-        <v>0.833333333333333</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="n">
-        <f aca="false">SUM(F2:F6)</f>
-        <v>200</v>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12" t="n">
+        <f aca="false">SUM(D2:D7)</f>
+        <v>1.20833333333333</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="n">
+        <f aca="false">SUM(F2:F7)</f>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#15] Added QA step in workflow with phpstan
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -438,7 +438,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
-        <v>45269</v>
+        <v>45270</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>0.541666666666667</v>
@@ -459,19 +459,81 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <f aca="false">(C9&lt;B9)+C9-B9</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <f aca="false">(D9*24)*E9</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>45272</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <f aca="false">(C10&lt;B10)+C10-B10</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <f aca="false">(D10*24)*E10</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
+        <v>45273</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="n">
+        <f aca="false">(C11&lt;B11)+C11-B11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9" t="n">
+        <f aca="false">(D11*24)*E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="n">
-        <f aca="false">SUM(D2:D8)</f>
-        <v>1.45833333333333</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="n">
-        <f aca="false">SUM(F2:F8)</f>
-        <v>350</v>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="n">
+        <f aca="false">SUM(D2:D11)</f>
+        <v>1.95833333333333</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13" t="n">
+        <f aca="false">SUM(F2:F11)</f>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#21] Forwarding filtering & ordering query params to the export action
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -525,19 +525,41 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <f aca="false">(C12&lt;B12)+C12-B12</f>
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <f aca="false">(D12*24)*E12</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12" t="n">
-        <f aca="false">SUM(D2:D11)</f>
-        <v>2.08333333333333</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13" t="n">
-        <f aca="false">SUM(F2:F11)</f>
-        <v>500</v>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="n">
+        <f aca="false">SUM(D2:D12)</f>
+        <v>2.16666666666667</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="n">
+        <f aca="false">SUM(F2:F12)</f>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#22] Add success and fail messages on import
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -547,19 +547,41 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="6" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <f aca="false">(C13&lt;B13)+C13-B13</f>
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <f aca="false">(D13*24)*E13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12" t="n">
-        <f aca="false">SUM(D2:D12)</f>
-        <v>2.16666666666667</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13" t="n">
-        <f aca="false">SUM(F2:F12)</f>
-        <v>520</v>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12" t="n">
+        <f aca="false">SUM(D2:D13)</f>
+        <v>2.41666666666667</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="n">
+        <f aca="false">SUM(F2:F13)</f>
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#27] Custom 2fa form
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -569,19 +569,41 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="6" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <f aca="false">(C14&lt;B14)+C14-B14</f>
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <f aca="false">(D14*24)*E14</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12" t="n">
-        <f aca="false">SUM(D2:D13)</f>
-        <v>2.41666666666667</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="n">
-        <f aca="false">SUM(F2:F13)</f>
-        <v>580</v>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12" t="n">
+        <f aca="false">SUM(D2:D14)</f>
+        <v>2.66666666666667</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="n">
+        <f aca="false">SUM(F2:F14)</f>
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#27] Added 2fa admin page for enable/disable
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -275,10 +275,10 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -576,18 +576,18 @@
         <v>0.583333333333333</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>0.833333333333333</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="D14" s="8" t="n">
         <f aca="false">(C14&lt;B14)+C14-B14</f>
-        <v>0.25</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>10</v>
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">(D14*24)*E14</f>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,12 +598,12 @@
       <c r="C15" s="11"/>
       <c r="D15" s="12" t="n">
         <f aca="false">SUM(D2:D14)</f>
-        <v>2.66666666666667</v>
+        <v>2.75</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13" t="n">
         <f aca="false">SUM(F2:F14)</f>
-        <v>640</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#37] Try using github actions var for env
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -591,19 +591,41 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="6" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <f aca="false">(C15&lt;B15)+C15-B15</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9" t="n">
+        <f aca="false">(D15*24)*E15</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12" t="n">
-        <f aca="false">SUM(D2:D14)</f>
-        <v>2.75</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="n">
-        <f aca="false">SUM(F2:F14)</f>
-        <v>660</v>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12" t="n">
+        <f aca="false">SUM(D2:D15)</f>
+        <v>3.08333333333333</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="n">
+        <f aca="false">SUM(F2:F15)</f>
+        <v>740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#41] Work on jwt auth. Need to set-up controller and authenticator.
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -613,19 +613,41 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="n">
+        <v>45282</v>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <f aca="false">(C16&lt;B16)+C16-B16</f>
+        <v>0.291666666666667</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="n">
+        <f aca="false">(D16*24)*E16</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12" t="n">
-        <f aca="false">SUM(D2:D15)</f>
-        <v>3.08333333333333</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13" t="n">
-        <f aca="false">SUM(F2:F15)</f>
-        <v>740</v>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12" t="n">
+        <f aca="false">SUM(D2:D16)</f>
+        <v>3.375</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="n">
+        <f aca="false">SUM(F2:F16)</f>
+        <v>810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#36] Added image for menu items
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -613,19 +613,63 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="n">
+        <v>45286</v>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <f aca="false">(C16&lt;B16)+C16-B16</f>
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="n">
+        <f aca="false">(D16*24)*E16</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <v>45287</v>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <f aca="false">(C17&lt;B17)+C17-B17</f>
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <f aca="false">(D17*24)*E17</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12" t="n">
-        <f aca="false">SUM(D2:D15)</f>
-        <v>3.08333333333333</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13" t="n">
-        <f aca="false">SUM(F2:F15)</f>
-        <v>740</v>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12" t="n">
+        <f aca="false">SUM(D2:D17)</f>
+        <v>3.375</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="n">
+        <f aca="false">SUM(F2:F17)</f>
+        <v>810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#41] Added ApiIntegration entity and CredentialsGenerator service
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -701,19 +701,41 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="6" t="n">
+        <v>45292</v>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <f aca="false">(C20&lt;B20)+C20-B20</f>
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9" t="n">
+        <f aca="false">(D20*24)*E20</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12" t="n">
-        <f aca="false">SUM(D2:D19)</f>
-        <v>3.875</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13" t="n">
-        <f aca="false">SUM(F2:F19)</f>
-        <v>930</v>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12" t="n">
+        <f aca="false">SUM(D2:D20)</f>
+        <v>4.08333333333333</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="n">
+        <f aca="false">SUM(F2:F20)</f>
+        <v>980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#41] Made clientId and clientSecret not change on save and readonly
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -319,11 +319,11 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="E2" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F2" s="9" t="n">
         <f aca="false">(D2*24)*E2</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,11 +341,11 @@
         <v>0.125</v>
       </c>
       <c r="E3" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F3" s="9" t="n">
         <f aca="false">(D3*24)*E3</f>
-        <v>30</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,11 +363,11 @@
         <v>0.125</v>
       </c>
       <c r="E4" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F4" s="9" t="n">
         <f aca="false">(D4*24)*E4</f>
-        <v>30</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,11 +385,11 @@
         <v>0.333333333333333</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F5" s="9" t="n">
         <f aca="false">(D5*24)*E5</f>
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,11 +407,11 @@
         <v>0.166666666666667</v>
       </c>
       <c r="E6" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F6" s="9" t="n">
         <f aca="false">(D6*24)*E6</f>
-        <v>40</v>
+        <v>54.0000000000001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,11 +429,11 @@
         <v>0.375</v>
       </c>
       <c r="E7" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F7" s="9" t="n">
         <f aca="false">(D7*24)*E7</f>
-        <v>90</v>
+        <v>121.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,11 +451,11 @@
         <v>0.25</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F8" s="9" t="n">
         <f aca="false">(D8*24)*E8</f>
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,11 +473,11 @@
         <v>0.166666666666667</v>
       </c>
       <c r="E9" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">(D9*24)*E9</f>
-        <v>40</v>
+        <v>54.0000000000001</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,11 +495,11 @@
         <v>0.333333333333333</v>
       </c>
       <c r="E10" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">(D10*24)*E10</f>
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,11 +517,11 @@
         <v>0.125</v>
       </c>
       <c r="E11" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">(D11*24)*E11</f>
-        <v>30</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,11 +539,11 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="E12" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">(D12*24)*E12</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,11 +561,11 @@
         <v>0.25</v>
       </c>
       <c r="E13" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">(D13*24)*E13</f>
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,11 +583,11 @@
         <v>0.333333333333333</v>
       </c>
       <c r="E14" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">(D14*24)*E14</f>
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,11 +605,11 @@
         <v>0.333333333333333</v>
       </c>
       <c r="E15" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">(D15*24)*E15</f>
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,11 +627,11 @@
         <v>0.291666666666667</v>
       </c>
       <c r="E16" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">(D16*24)*E16</f>
-        <v>70</v>
+        <v>94.5000000000001</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,11 +649,11 @@
         <v>0.208333333333333</v>
       </c>
       <c r="E17" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">(D17*24)*E17</f>
-        <v>50</v>
+        <v>67.4999999999999</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,11 +671,11 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="E18" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">(D18*24)*E18</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,11 +693,11 @@
         <v>0.208333333333333</v>
       </c>
       <c r="E19" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">(D19*24)*E19</f>
-        <v>50</v>
+        <v>67.4999999999999</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,27 +715,71 @@
         <v>0.208333333333333</v>
       </c>
       <c r="E20" s="9" t="n">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">(D20*24)*E20</f>
-        <v>50</v>
+        <v>67.4999999999999</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6" t="n">
+        <v>45311</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="D21" s="8" t="n">
+        <f aca="false">(C21&lt;B21)+C21-B21</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E21" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F21" s="9" t="n">
+        <f aca="false">(D21*24)*E21</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="n">
+        <v>45312</v>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D22" s="8" t="n">
+        <f aca="false">(C22&lt;B22)+C22-B22</f>
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E22" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F22" s="9" t="n">
+        <f aca="false">(D22*24)*E22</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12" t="n">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12" t="n">
         <f aca="false">SUM(D2:D20)</f>
         <v>4.08333333333333</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="n">
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="n">
         <f aca="false">SUM(F2:F20)</f>
-        <v>980</v>
+        <v>1323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#45] Bookings - able to validate and save on front form submission
</commit_message>
<xml_diff>
--- a/working-hours.xlsx
+++ b/working-hours.xlsx
@@ -272,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.54"/>
@@ -767,19 +767,151 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="6" t="n">
+        <v>45316</v>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D23" s="8" t="n">
+        <f aca="false">(C23&lt;B23)+C23-B23</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E23" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F23" s="9" t="n">
+        <f aca="false">(D23*24)*E23</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
+        <v>45318</v>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C24" s="7" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D24" s="8" t="n">
+        <f aca="false">(C24&lt;B24)+C24-B24</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E24" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F24" s="9" t="n">
+        <f aca="false">(D24*24)*E24</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
+        <v>45319</v>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C25" s="7" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <f aca="false">(C25&lt;B25)+C25-B25</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E25" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F25" s="9" t="n">
+        <f aca="false">(D25*24)*E25</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
+        <v>45320</v>
+      </c>
+      <c r="B26" s="7" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C26" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D26" s="8" t="n">
+        <f aca="false">(C26&lt;B26)+C26-B26</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E26" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F26" s="9" t="n">
+        <f aca="false">(D26*24)*E26</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
+        <v>45321</v>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D27" s="8" t="n">
+        <f aca="false">(C27&lt;B27)+C27-B27</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E27" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F27" s="9" t="n">
+        <f aca="false">(D27*24)*E27</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
+        <v>45322</v>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="D28" s="8" t="n">
+        <f aca="false">(C28&lt;B28)+C28-B28</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <f aca="false">(D28*24)*E28</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12" t="n">
-        <f aca="false">SUM(D2:D20)</f>
-        <v>4.08333333333333</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="n">
-        <f aca="false">SUM(F2:F20)</f>
-        <v>1323</v>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12" t="n">
+        <f aca="false">SUM(D2:D28)</f>
+        <v>5.83333333333333</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13" t="n">
+        <f aca="false">SUM(F2:F28)</f>
+        <v>1890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>